<commit_message>
test revised function:sub,tram,bus_stations;try to solve metro51
</commit_message>
<xml_diff>
--- a/notebooks/city_bus_new_nodes_transfer_all.xlsx
+++ b/notebooks/city_bus_new_nodes_transfer_all.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -561,7 +561,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'62', '25', '65', '5', '15'}</t>
+          <t>{'25', '15', '62', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{'5', '246', '15', '65'}</t>
+          <t>{'246', '15', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>{'2', '15', '24', '62'}</t>
+          <t>{'15', '2', '62', '24'}</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>{'24', '62', '2', '50', '246', '15', '51'}</t>
+          <t>{'24', '15', '62', '246', '51', '50', '2'}</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>{'2', '15', '62'}</t>
+          <t>{'15', '2', '62'}</t>
         </is>
       </c>
     </row>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>{'247', '15', '1', '17'}</t>
+          <t>{'247', '15', '17', '1'}</t>
         </is>
       </c>
     </row>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>{'17', '18', '7', '247', '15'}</t>
+          <t>{'247', '15', '7', '17', '18'}</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{'18', '247', '15', '7'}</t>
+          <t>{'247', '18', '15', '7'}</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>{'13', '18', '7', '247', '15'}</t>
+          <t>{'13', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>{'13', '19', '18', '7', '247', '15'}</t>
+          <t>{'13', '19', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>{'7', '15'}</t>
+          <t>{'15', '7'}</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>{'21', '247', '15', '7'}</t>
+          <t>{'247', '15', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>{'21', '247', '15', '7'}</t>
+          <t>{'247', '15', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>{'13', '19', '18', '7', '247', '15'}</t>
+          <t>{'13', '19', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>{'13', '18', '7', '247', '15'}</t>
+          <t>{'13', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>{'18', '247', '15', '7'}</t>
+          <t>{'247', '18', '15', '7'}</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>{'17', '18', '7', '247', '15'}</t>
+          <t>{'247', '15', '7', '17', '18'}</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>{'247', '15', '1', '17'}</t>
+          <t>{'247', '15', '17', '1'}</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>{'5', '246', '15', '65'}</t>
+          <t>{'246', '15', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>{'62', '25', '65', '5', '15'}</t>
+          <t>{'25', '15', '62', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>{'18', '247', '2'}</t>
+          <t>{'247', '18', '2'}</t>
         </is>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>{'17', '62', '18', '2', '1', '247'}</t>
+          <t>{'247', '62', '17', '1', '18', '2'}</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr">
         <is>
-          <t>{'18', '247', '62'}</t>
+          <t>{'247', '18', '62'}</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>{'17', '18', '2', '1', '63'}</t>
+          <t>{'63', '17', '1', '18', '2'}</t>
         </is>
       </c>
     </row>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>{'13', '18', '7', '247', '15'}</t>
+          <t>{'13', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>{'18', '247', '13'}</t>
+          <t>{'247', '18', '13'}</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>{'18', '247', '19', '13'}</t>
+          <t>{'247', '18', '19', '13'}</t>
         </is>
       </c>
     </row>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>{'13', '19', '18', '7', '247', '15'}</t>
+          <t>{'13', '19', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr">
         <is>
-          <t>{'18', '21', '22'}</t>
+          <t>{'22', '18', '21'}</t>
         </is>
       </c>
     </row>
@@ -3613,7 +3613,7 @@
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr">
         <is>
-          <t>{'18', '21', '22'}</t>
+          <t>{'22', '18', '21'}</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr">
         <is>
-          <t>{'18', '21', '22'}</t>
+          <t>{'22', '18', '21'}</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr">
         <is>
-          <t>{'21', '54', '48', '53', '18', '43', '22', '52', '51'}</t>
+          <t>{'22', '54', '53', '48', '18', '51', '21', '52', '43'}</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr">
         <is>
-          <t>{'21', '54', '48', '53', '18', '43', '22', '52', '51'}</t>
+          <t>{'22', '54', '53', '48', '18', '51', '21', '52', '43'}</t>
         </is>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr">
         <is>
-          <t>{'18', '21', '22'}</t>
+          <t>{'22', '18', '21'}</t>
         </is>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
       <c r="M60" t="inlineStr"/>
       <c r="N60" t="inlineStr">
         <is>
-          <t>{'18', '21', '22'}</t>
+          <t>{'22', '18', '21'}</t>
         </is>
       </c>
     </row>
@@ -3957,7 +3957,7 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr">
         <is>
-          <t>{'18', '21', '22'}</t>
+          <t>{'22', '18', '21'}</t>
         </is>
       </c>
     </row>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>{'13', '19', '18', '7', '247', '15'}</t>
+          <t>{'13', '19', '247', '15', '7', '18'}</t>
         </is>
       </c>
     </row>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>{'18', '247', '13'}</t>
+          <t>{'247', '18', '13'}</t>
         </is>
       </c>
     </row>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>{'18', '17', '7'}</t>
+          <t>{'18', '7', '17'}</t>
         </is>
       </c>
     </row>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>{'17', '18', '2', '1', '63'}</t>
+          <t>{'63', '17', '1', '18', '2'}</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       <c r="M78" t="inlineStr"/>
       <c r="N78" t="inlineStr">
         <is>
-          <t>{'18', '247', '62'}</t>
+          <t>{'247', '18', '62'}</t>
         </is>
       </c>
     </row>
@@ -4953,7 +4953,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>{'17', '62', '18', '2', '1', '247'}</t>
+          <t>{'247', '62', '17', '1', '18', '2'}</t>
         </is>
       </c>
     </row>
@@ -5013,7 +5013,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>{'18', '247', '2'}</t>
+          <t>{'247', '18', '2'}</t>
         </is>
       </c>
     </row>
@@ -5461,7 +5461,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>{'21', '369', '7'}</t>
+          <t>{'369', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -5633,7 +5633,7 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>{'21', '50', '7', '51'}</t>
+          <t>{'50', '51', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>{'21', '247', '15', '7'}</t>
+          <t>{'247', '15', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -5749,7 +5749,7 @@
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr">
         <is>
-          <t>{'21', '247'}</t>
+          <t>{'247', '21'}</t>
         </is>
       </c>
     </row>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>{'21', '247', '19'}</t>
+          <t>{'19', '247', '21'}</t>
         </is>
       </c>
     </row>
@@ -6181,7 +6181,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>{'21', '247', '19'}</t>
+          <t>{'19', '247', '21'}</t>
         </is>
       </c>
     </row>
@@ -6237,7 +6237,7 @@
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr">
         <is>
-          <t>{'21', '247'}</t>
+          <t>{'247', '21'}</t>
         </is>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>{'21', '50', '7', '51'}</t>
+          <t>{'50', '51', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -6469,7 +6469,7 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>{'21', '369', '7'}</t>
+          <t>{'369', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -6813,7 +6813,7 @@
       <c r="M112" t="inlineStr"/>
       <c r="N112" t="inlineStr">
         <is>
-          <t>{'36', '22'}</t>
+          <t>{'22', '36'}</t>
         </is>
       </c>
     </row>
@@ -7077,7 +7077,7 @@
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr">
         <is>
-          <t>{'48', '22'}</t>
+          <t>{'22', '48'}</t>
         </is>
       </c>
     </row>
@@ -7241,7 +7241,7 @@
       <c r="M120" t="inlineStr"/>
       <c r="N120" t="inlineStr">
         <is>
-          <t>{'21', '54', '48', '53', '18', '43', '22', '52', '51'}</t>
+          <t>{'22', '54', '53', '48', '18', '51', '21', '52', '43'}</t>
         </is>
       </c>
     </row>
@@ -7301,7 +7301,7 @@
       <c r="M121" t="inlineStr"/>
       <c r="N121" t="inlineStr">
         <is>
-          <t>{'54', '53', '43', '22', '52', '51'}</t>
+          <t>{'22', '54', '53', '51', '52', '43'}</t>
         </is>
       </c>
     </row>
@@ -7357,7 +7357,7 @@
       <c r="M122" t="inlineStr"/>
       <c r="N122" t="inlineStr">
         <is>
-          <t>{'43', '246', '22'}</t>
+          <t>{'22', '246', '43'}</t>
         </is>
       </c>
     </row>
@@ -7517,7 +7517,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>{'7', '22'}</t>
+          <t>{'22', '7'}</t>
         </is>
       </c>
     </row>
@@ -7625,7 +7625,7 @@
       <c r="M127" t="inlineStr"/>
       <c r="N127" t="inlineStr">
         <is>
-          <t>{'65', '22'}</t>
+          <t>{'22', '65'}</t>
         </is>
       </c>
     </row>
@@ -7681,7 +7681,7 @@
       <c r="M128" t="inlineStr"/>
       <c r="N128" t="inlineStr">
         <is>
-          <t>{'65', '22'}</t>
+          <t>{'22', '65'}</t>
         </is>
       </c>
     </row>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>{'14', '65', '22'}</t>
+          <t>{'22', '14', '65'}</t>
         </is>
       </c>
     </row>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>{'14', '40', '245', '37', '240', '3', '22'}</t>
+          <t>{'22', '14', '240', '245', '37', '40', '3'}</t>
         </is>
       </c>
     </row>
@@ -7861,7 +7861,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>{'41', '40', '245', '37', '240', '3', '22', '1'}</t>
+          <t>{'22', '240', '245', '37', '1', '41', '40', '3'}</t>
         </is>
       </c>
     </row>
@@ -7921,7 +7921,7 @@
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>{'41', '40', '245', '37', '240', '3', '22', '1'}</t>
+          <t>{'22', '240', '245', '37', '1', '41', '40', '3'}</t>
         </is>
       </c>
     </row>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>{'7', '22'}</t>
+          <t>{'22', '7'}</t>
         </is>
       </c>
     </row>
@@ -8189,7 +8189,7 @@
       <c r="M137" t="inlineStr"/>
       <c r="N137" t="inlineStr">
         <is>
-          <t>{'43', '246', '22'}</t>
+          <t>{'22', '246', '43'}</t>
         </is>
       </c>
     </row>
@@ -8245,7 +8245,7 @@
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="inlineStr">
         <is>
-          <t>{'43', '22'}</t>
+          <t>{'22', '43'}</t>
         </is>
       </c>
     </row>
@@ -8305,7 +8305,7 @@
       <c r="M139" t="inlineStr"/>
       <c r="N139" t="inlineStr">
         <is>
-          <t>{'54', '53', '43', '22', '52', '51'}</t>
+          <t>{'22', '54', '53', '51', '52', '43'}</t>
         </is>
       </c>
     </row>
@@ -8465,7 +8465,7 @@
       <c r="M142" t="inlineStr"/>
       <c r="N142" t="inlineStr">
         <is>
-          <t>{'48', '22'}</t>
+          <t>{'22', '48'}</t>
         </is>
       </c>
     </row>
@@ -8729,7 +8729,7 @@
       <c r="M147" t="inlineStr"/>
       <c r="N147" t="inlineStr">
         <is>
-          <t>{'36', '22'}</t>
+          <t>{'22', '36'}</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9313,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -9853,7 +9853,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>{'14', '40', '245', '37', '240', '3', '22'}</t>
+          <t>{'22', '14', '240', '245', '37', '40', '3'}</t>
         </is>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       <c r="M169" t="inlineStr"/>
       <c r="N169" t="inlineStr">
         <is>
-          <t>{'240', '65', '40'}</t>
+          <t>{'40', '240', '65'}</t>
         </is>
       </c>
     </row>
@@ -9965,7 +9965,7 @@
       <c r="M170" t="inlineStr"/>
       <c r="N170" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10021,7 +10021,7 @@
       <c r="M171" t="inlineStr"/>
       <c r="N171" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10077,7 +10077,7 @@
       <c r="M172" t="inlineStr"/>
       <c r="N172" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10133,7 +10133,7 @@
       <c r="M173" t="inlineStr"/>
       <c r="N173" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10189,7 +10189,7 @@
       <c r="M174" t="inlineStr"/>
       <c r="N174" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10245,7 +10245,7 @@
       <c r="M175" t="inlineStr"/>
       <c r="N175" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10301,7 +10301,7 @@
       <c r="M176" t="inlineStr"/>
       <c r="N176" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10361,7 +10361,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>{'240', '41', '19', '40'}</t>
+          <t>{'19', '40', '240', '41'}</t>
         </is>
       </c>
     </row>
@@ -10417,7 +10417,7 @@
       <c r="M178" t="inlineStr"/>
       <c r="N178" t="inlineStr">
         <is>
-          <t>{'240', '41', '40'}</t>
+          <t>{'40', '240', '41'}</t>
         </is>
       </c>
     </row>
@@ -10473,7 +10473,7 @@
       <c r="M179" t="inlineStr"/>
       <c r="N179" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10529,7 +10529,7 @@
       <c r="M180" t="inlineStr"/>
       <c r="N180" t="inlineStr">
         <is>
-          <t>{'40', '245', '37', '240', '65'}</t>
+          <t>{'240', '245', '37', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -10585,7 +10585,7 @@
       <c r="M181" t="inlineStr"/>
       <c r="N181" t="inlineStr">
         <is>
-          <t>{'40', '245', '37', '240', '65'}</t>
+          <t>{'240', '245', '37', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -10645,7 +10645,7 @@
       <c r="M182" t="inlineStr"/>
       <c r="N182" t="inlineStr">
         <is>
-          <t>{'40', '245', '54', '53', '62', '240', '37', '65', '51'}</t>
+          <t>{'240', '54', '245', '53', '62', '37', '51', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -10705,7 +10705,7 @@
       <c r="M183" t="inlineStr"/>
       <c r="N183" t="inlineStr">
         <is>
-          <t>{'40', '245', '54', '53', '62', '240', '37', '65', '51'}</t>
+          <t>{'240', '54', '245', '53', '62', '37', '51', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -10761,7 +10761,7 @@
       <c r="M184" t="inlineStr"/>
       <c r="N184" t="inlineStr">
         <is>
-          <t>{'40', '245', '37', '240', '65'}</t>
+          <t>{'240', '245', '37', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -10817,7 +10817,7 @@
       <c r="M185" t="inlineStr"/>
       <c r="N185" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -10873,7 +10873,7 @@
       <c r="M186" t="inlineStr"/>
       <c r="N186" t="inlineStr">
         <is>
-          <t>{'240', '41', '40'}</t>
+          <t>{'40', '240', '41'}</t>
         </is>
       </c>
     </row>
@@ -10933,7 +10933,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>{'240', '41', '19', '40'}</t>
+          <t>{'19', '40', '240', '41'}</t>
         </is>
       </c>
     </row>
@@ -10989,7 +10989,7 @@
       <c r="M188" t="inlineStr"/>
       <c r="N188" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -11045,7 +11045,7 @@
       <c r="M189" t="inlineStr"/>
       <c r="N189" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -11101,7 +11101,7 @@
       <c r="M190" t="inlineStr"/>
       <c r="N190" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -11157,7 +11157,7 @@
       <c r="M191" t="inlineStr"/>
       <c r="N191" t="inlineStr">
         <is>
-          <t>{'240', '40'}</t>
+          <t>{'40', '240'}</t>
         </is>
       </c>
     </row>
@@ -11213,7 +11213,7 @@
       <c r="M192" t="inlineStr"/>
       <c r="N192" t="inlineStr">
         <is>
-          <t>{'240', '65', '40'}</t>
+          <t>{'40', '240', '65'}</t>
         </is>
       </c>
     </row>
@@ -11585,7 +11585,7 @@
       <c r="M199" t="inlineStr"/>
       <c r="N199" t="inlineStr">
         <is>
-          <t>{'36', '34', '245'}</t>
+          <t>{'36', '245', '34'}</t>
         </is>
       </c>
     </row>
@@ -11641,7 +11641,7 @@
       <c r="M200" t="inlineStr"/>
       <c r="N200" t="inlineStr">
         <is>
-          <t>{'36', '34', '245'}</t>
+          <t>{'36', '245', '34'}</t>
         </is>
       </c>
     </row>
@@ -11701,7 +11701,7 @@
       <c r="M201" t="inlineStr"/>
       <c r="N201" t="inlineStr">
         <is>
-          <t>{'34', '245', '37', '36', '38', '52'}</t>
+          <t>{'38', '245', '34', '37', '52', '36'}</t>
         </is>
       </c>
     </row>
@@ -11757,7 +11757,7 @@
       <c r="M202" t="inlineStr"/>
       <c r="N202" t="inlineStr">
         <is>
-          <t>{'37', '34', '245'}</t>
+          <t>{'245', '34', '37'}</t>
         </is>
       </c>
     </row>
@@ -11813,7 +11813,7 @@
       <c r="M203" t="inlineStr"/>
       <c r="N203" t="inlineStr">
         <is>
-          <t>{'38', '37', '34', '245'}</t>
+          <t>{'38', '245', '34', '37'}</t>
         </is>
       </c>
     </row>
@@ -11869,7 +11869,7 @@
       <c r="M204" t="inlineStr"/>
       <c r="N204" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -11925,7 +11925,7 @@
       <c r="M205" t="inlineStr"/>
       <c r="N205" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11981,7 @@
       <c r="M206" t="inlineStr"/>
       <c r="N206" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12037,7 +12037,7 @@
       <c r="M207" t="inlineStr"/>
       <c r="N207" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12093,7 +12093,7 @@
       <c r="M208" t="inlineStr"/>
       <c r="N208" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12149,7 +12149,7 @@
       <c r="M209" t="inlineStr"/>
       <c r="N209" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12209,7 +12209,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>{'26', '37', '245'}</t>
+          <t>{'26', '245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12269,7 +12269,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>{'14', '3', '37', '245'}</t>
+          <t>{'14', '3', '245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12329,7 +12329,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>{'14', '3', '37', '245'}</t>
+          <t>{'14', '3', '245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12389,7 +12389,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>{'41', '245', '37', '3', '1'}</t>
+          <t>{'245', '1', '37', '41', '3'}</t>
         </is>
       </c>
     </row>
@@ -12449,7 +12449,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>{'41', '245', '37', '3', '1'}</t>
+          <t>{'245', '1', '37', '41', '3'}</t>
         </is>
       </c>
     </row>
@@ -12505,7 +12505,7 @@
       <c r="M215" t="inlineStr"/>
       <c r="N215" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12561,7 +12561,7 @@
       <c r="M216" t="inlineStr"/>
       <c r="N216" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12617,7 +12617,7 @@
       <c r="M217" t="inlineStr"/>
       <c r="N217" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -12677,7 +12677,7 @@
       <c r="M218" t="inlineStr"/>
       <c r="N218" t="inlineStr">
         <is>
-          <t>{'40', '245', '54', '53', '62', '240', '37', '65', '51'}</t>
+          <t>{'240', '54', '245', '53', '62', '37', '51', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -12737,7 +12737,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>{'62', '65', '12', '245'}</t>
+          <t>{'65', '12', '245', '62'}</t>
         </is>
       </c>
     </row>
@@ -12797,7 +12797,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -12857,7 +12857,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -12917,7 +12917,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -12981,7 +12981,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>{'52', '65', '4', '245'}</t>
+          <t>{'52', '4', '245', '65'}</t>
         </is>
       </c>
     </row>
@@ -13037,7 +13037,7 @@
       <c r="M224" t="inlineStr"/>
       <c r="N224" t="inlineStr">
         <is>
-          <t>{'245', '267', '369', '247', '246'}</t>
+          <t>{'245', '247', '369', '267', '246'}</t>
         </is>
       </c>
     </row>
@@ -13093,7 +13093,7 @@
       <c r="M225" t="inlineStr"/>
       <c r="N225" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13149,7 +13149,7 @@
       <c r="M226" t="inlineStr"/>
       <c r="N226" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13205,7 +13205,7 @@
       <c r="M227" t="inlineStr"/>
       <c r="N227" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13261,7 +13261,7 @@
       <c r="M228" t="inlineStr"/>
       <c r="N228" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13317,7 +13317,7 @@
       <c r="M229" t="inlineStr"/>
       <c r="N229" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13373,7 +13373,7 @@
       <c r="M230" t="inlineStr"/>
       <c r="N230" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13429,7 +13429,7 @@
       <c r="M231" t="inlineStr"/>
       <c r="N231" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -13765,7 +13765,7 @@
       <c r="M237" t="inlineStr"/>
       <c r="N237" t="inlineStr">
         <is>
-          <t>{'43', '246', '65'}</t>
+          <t>{'246', '43', '65'}</t>
         </is>
       </c>
     </row>
@@ -13825,7 +13825,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>{'43', '246', '65', '7'}</t>
+          <t>{'246', '43', '7', '65'}</t>
         </is>
       </c>
     </row>
@@ -13885,7 +13885,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>{'43', '246', '65', '7'}</t>
+          <t>{'246', '43', '7', '65'}</t>
         </is>
       </c>
     </row>
@@ -13941,7 +13941,7 @@
       <c r="M240" t="inlineStr"/>
       <c r="N240" t="inlineStr">
         <is>
-          <t>{'43', '246'}</t>
+          <t>{'246', '43'}</t>
         </is>
       </c>
     </row>
@@ -13997,7 +13997,7 @@
       <c r="M241" t="inlineStr"/>
       <c r="N241" t="inlineStr">
         <is>
-          <t>{'43', '246'}</t>
+          <t>{'246', '43'}</t>
         </is>
       </c>
     </row>
@@ -14057,7 +14057,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>{'43', '246', '26'}</t>
+          <t>{'246', '26', '43'}</t>
         </is>
       </c>
     </row>
@@ -14113,7 +14113,7 @@
       <c r="M243" t="inlineStr"/>
       <c r="N243" t="inlineStr">
         <is>
-          <t>{'43', '246'}</t>
+          <t>{'246', '43'}</t>
         </is>
       </c>
     </row>
@@ -14229,7 +14229,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>{'54', '19', '53', '1', '7', '246', '51'}</t>
+          <t>{'54', '53', '19', '7', '1', '246', '51'}</t>
         </is>
       </c>
     </row>
@@ -14397,7 +14397,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>{'246', '12'}</t>
+          <t>{'12', '246'}</t>
         </is>
       </c>
     </row>
@@ -14453,7 +14453,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>{'246', '12'}</t>
+          <t>{'12', '246'}</t>
         </is>
       </c>
     </row>
@@ -14513,7 +14513,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>{'246', '65', '12'}</t>
+          <t>{'12', '246', '65'}</t>
         </is>
       </c>
     </row>
@@ -14629,7 +14629,7 @@
       </c>
       <c r="N252" t="inlineStr">
         <is>
-          <t>{'5', '246', '65', '24'}</t>
+          <t>{'246', '5', '24', '65'}</t>
         </is>
       </c>
     </row>
@@ -14689,7 +14689,7 @@
       </c>
       <c r="N253" t="inlineStr">
         <is>
-          <t>{'5', '246', '65', '24'}</t>
+          <t>{'246', '5', '24', '65'}</t>
         </is>
       </c>
     </row>
@@ -14749,7 +14749,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>{'5', '246', '15', '65'}</t>
+          <t>{'246', '15', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -14913,7 +14913,7 @@
       </c>
       <c r="N257" t="inlineStr">
         <is>
-          <t>{'62', '246', '24', '461'}</t>
+          <t>{'246', '461', '24', '62'}</t>
         </is>
       </c>
     </row>
@@ -14973,7 +14973,7 @@
       </c>
       <c r="N258" t="inlineStr">
         <is>
-          <t>{'246', '24', '62'}</t>
+          <t>{'246', '62', '24'}</t>
         </is>
       </c>
     </row>
@@ -15037,7 +15037,7 @@
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>{'24', '62', '2', '50', '246', '15', '51'}</t>
+          <t>{'24', '15', '62', '246', '51', '50', '2'}</t>
         </is>
       </c>
     </row>
@@ -15257,7 +15257,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>{'369', '247', '2'}</t>
+          <t>{'247', '369', '2'}</t>
         </is>
       </c>
     </row>
@@ -15313,7 +15313,7 @@
       <c r="M264" t="inlineStr"/>
       <c r="N264" t="inlineStr">
         <is>
-          <t>{'369', '247'}</t>
+          <t>{'247', '369'}</t>
         </is>
       </c>
     </row>
@@ -15369,7 +15369,7 @@
       <c r="M265" t="inlineStr"/>
       <c r="N265" t="inlineStr">
         <is>
-          <t>{'68', '267'}</t>
+          <t>{'267', '68'}</t>
         </is>
       </c>
     </row>
@@ -15425,7 +15425,7 @@
       <c r="M266" t="inlineStr"/>
       <c r="N266" t="inlineStr">
         <is>
-          <t>{'68', '267'}</t>
+          <t>{'267', '68'}</t>
         </is>
       </c>
     </row>
@@ -15481,7 +15481,7 @@
       <c r="M267" t="inlineStr"/>
       <c r="N267" t="inlineStr">
         <is>
-          <t>{'245', '267', '369', '247', '246'}</t>
+          <t>{'245', '247', '369', '267', '246'}</t>
         </is>
       </c>
     </row>
@@ -15537,7 +15537,7 @@
       <c r="M268" t="inlineStr"/>
       <c r="N268" t="inlineStr">
         <is>
-          <t>{'68', '267'}</t>
+          <t>{'267', '68'}</t>
         </is>
       </c>
     </row>
@@ -15593,7 +15593,7 @@
       <c r="M269" t="inlineStr"/>
       <c r="N269" t="inlineStr">
         <is>
-          <t>{'38', '37', '34', '245'}</t>
+          <t>{'38', '245', '34', '37'}</t>
         </is>
       </c>
     </row>
@@ -15761,7 +15761,7 @@
       <c r="M272" t="inlineStr"/>
       <c r="N272" t="inlineStr">
         <is>
-          <t>{'37', '34', '245'}</t>
+          <t>{'245', '34', '37'}</t>
         </is>
       </c>
     </row>
@@ -15821,7 +15821,7 @@
       <c r="M273" t="inlineStr"/>
       <c r="N273" t="inlineStr">
         <is>
-          <t>{'34', '245', '37', '36', '38', '52'}</t>
+          <t>{'38', '245', '34', '37', '52', '36'}</t>
         </is>
       </c>
     </row>
@@ -15877,7 +15877,7 @@
       <c r="M274" t="inlineStr"/>
       <c r="N274" t="inlineStr">
         <is>
-          <t>{'36', '34', '245'}</t>
+          <t>{'36', '245', '34'}</t>
         </is>
       </c>
     </row>
@@ -15933,7 +15933,7 @@
       <c r="M275" t="inlineStr"/>
       <c r="N275" t="inlineStr">
         <is>
-          <t>{'36', '34', '245'}</t>
+          <t>{'36', '245', '34'}</t>
         </is>
       </c>
     </row>
@@ -16581,7 +16581,7 @@
       <c r="M287" t="inlineStr"/>
       <c r="N287" t="inlineStr">
         <is>
-          <t>{'35', '52', '34'}</t>
+          <t>{'52', '35', '34'}</t>
         </is>
       </c>
     </row>
@@ -16641,7 +16641,7 @@
       <c r="M288" t="inlineStr"/>
       <c r="N288" t="inlineStr">
         <is>
-          <t>{'35', '52', '34'}</t>
+          <t>{'52', '35', '34'}</t>
         </is>
       </c>
     </row>
@@ -19241,7 +19241,7 @@
       <c r="M336" t="inlineStr"/>
       <c r="N336" t="inlineStr">
         <is>
-          <t>{'34', '245', '37', '36', '38', '52'}</t>
+          <t>{'38', '245', '34', '37', '52', '36'}</t>
         </is>
       </c>
     </row>
@@ -19621,7 +19621,7 @@
       </c>
       <c r="N343" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -19889,7 +19889,7 @@
       <c r="M348" t="inlineStr"/>
       <c r="N348" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -19945,7 +19945,7 @@
       <c r="M349" t="inlineStr"/>
       <c r="N349" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -20001,7 +20001,7 @@
       <c r="M350" t="inlineStr"/>
       <c r="N350" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -20057,7 +20057,7 @@
       <c r="M351" t="inlineStr"/>
       <c r="N351" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -20113,7 +20113,7 @@
       <c r="M352" t="inlineStr"/>
       <c r="N352" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -20169,7 +20169,7 @@
       <c r="M353" t="inlineStr"/>
       <c r="N353" t="inlineStr">
         <is>
-          <t>{'369', '247'}</t>
+          <t>{'247', '369'}</t>
         </is>
       </c>
     </row>
@@ -20229,7 +20229,7 @@
       </c>
       <c r="N354" t="inlineStr">
         <is>
-          <t>{'369', '247', '2'}</t>
+          <t>{'247', '369', '2'}</t>
         </is>
       </c>
     </row>
@@ -20397,7 +20397,7 @@
       </c>
       <c r="N357" t="inlineStr">
         <is>
-          <t>{'369', '17', '63'}</t>
+          <t>{'369', '63', '17'}</t>
         </is>
       </c>
     </row>
@@ -20453,7 +20453,7 @@
       <c r="M358" t="inlineStr"/>
       <c r="N358" t="inlineStr">
         <is>
-          <t>{'369', '61', '63'}</t>
+          <t>{'369', '63', '61'}</t>
         </is>
       </c>
     </row>
@@ -20681,7 +20681,7 @@
       </c>
       <c r="N362" t="inlineStr">
         <is>
-          <t>{'21', '369', '7'}</t>
+          <t>{'369', '21', '7'}</t>
         </is>
       </c>
     </row>
@@ -20745,7 +20745,7 @@
       </c>
       <c r="N363" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -20965,7 +20965,7 @@
       <c r="M367" t="inlineStr"/>
       <c r="N367" t="inlineStr">
         <is>
-          <t>{'369', '61', '63'}</t>
+          <t>{'369', '63', '61'}</t>
         </is>
       </c>
     </row>
@@ -21025,7 +21025,7 @@
       </c>
       <c r="N368" t="inlineStr">
         <is>
-          <t>{'369', '17', '63'}</t>
+          <t>{'369', '63', '17'}</t>
         </is>
       </c>
     </row>
@@ -21189,7 +21189,7 @@
       <c r="M371" t="inlineStr"/>
       <c r="N371" t="inlineStr">
         <is>
-          <t>{'369', '247', '246', '245'}</t>
+          <t>{'247', '246', '369', '245'}</t>
         </is>
       </c>
     </row>
@@ -21249,7 +21249,7 @@
       <c r="M372" t="inlineStr"/>
       <c r="N372" t="inlineStr">
         <is>
-          <t>{'34', '245', '37', '36', '38', '52'}</t>
+          <t>{'38', '245', '34', '37', '52', '36'}</t>
         </is>
       </c>
     </row>
@@ -21309,7 +21309,7 @@
       <c r="M373" t="inlineStr"/>
       <c r="N373" t="inlineStr">
         <is>
-          <t>{'40', '245', '54', '53', '62', '240', '37', '65', '51'}</t>
+          <t>{'240', '54', '245', '53', '62', '37', '51', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -21365,7 +21365,7 @@
       <c r="M374" t="inlineStr"/>
       <c r="N374" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21421,7 +21421,7 @@
       <c r="M375" t="inlineStr"/>
       <c r="N375" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21481,7 +21481,7 @@
       </c>
       <c r="N376" t="inlineStr">
         <is>
-          <t>{'41', '245', '37', '3', '1'}</t>
+          <t>{'245', '1', '37', '41', '3'}</t>
         </is>
       </c>
     </row>
@@ -21541,7 +21541,7 @@
       </c>
       <c r="N377" t="inlineStr">
         <is>
-          <t>{'41', '245', '37', '3', '1'}</t>
+          <t>{'245', '1', '37', '41', '3'}</t>
         </is>
       </c>
     </row>
@@ -21601,7 +21601,7 @@
       </c>
       <c r="N378" t="inlineStr">
         <is>
-          <t>{'14', '40', '245', '37', '240', '3', '22'}</t>
+          <t>{'22', '14', '240', '245', '37', '40', '3'}</t>
         </is>
       </c>
     </row>
@@ -21661,7 +21661,7 @@
       </c>
       <c r="N379" t="inlineStr">
         <is>
-          <t>{'14', '3', '37', '245'}</t>
+          <t>{'14', '3', '245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21721,7 +21721,7 @@
       </c>
       <c r="N380" t="inlineStr">
         <is>
-          <t>{'14', '3', '37', '245'}</t>
+          <t>{'14', '3', '245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21781,7 +21781,7 @@
       </c>
       <c r="N381" t="inlineStr">
         <is>
-          <t>{'26', '37', '245'}</t>
+          <t>{'26', '245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21837,7 +21837,7 @@
       <c r="M382" t="inlineStr"/>
       <c r="N382" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21893,7 +21893,7 @@
       <c r="M383" t="inlineStr"/>
       <c r="N383" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -21949,7 +21949,7 @@
       <c r="M384" t="inlineStr"/>
       <c r="N384" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -22005,7 +22005,7 @@
       <c r="M385" t="inlineStr"/>
       <c r="N385" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -22061,7 +22061,7 @@
       <c r="M386" t="inlineStr"/>
       <c r="N386" t="inlineStr">
         <is>
-          <t>{'37', '245'}</t>
+          <t>{'245', '37'}</t>
         </is>
       </c>
     </row>
@@ -22333,7 +22333,7 @@
       <c r="M391" t="inlineStr"/>
       <c r="N391" t="inlineStr">
         <is>
-          <t>{'34', '245', '37', '36', '38', '52'}</t>
+          <t>{'38', '245', '34', '37', '52', '36'}</t>
         </is>
       </c>
     </row>
@@ -23381,7 +23381,7 @@
       <c r="M411" t="inlineStr"/>
       <c r="N411" t="inlineStr">
         <is>
-          <t>{'41', '54', '50'}</t>
+          <t>{'50', '41', '54'}</t>
         </is>
       </c>
     </row>
@@ -23545,7 +23545,7 @@
       </c>
       <c r="N414" t="inlineStr">
         <is>
-          <t>{'41', '19'}</t>
+          <t>{'19', '41'}</t>
         </is>
       </c>
     </row>
@@ -23601,7 +23601,7 @@
       </c>
       <c r="N415" t="inlineStr">
         <is>
-          <t>{'41', '19'}</t>
+          <t>{'19', '41'}</t>
         </is>
       </c>
     </row>
@@ -23657,7 +23657,7 @@
       </c>
       <c r="N416" t="inlineStr">
         <is>
-          <t>{'41', '19'}</t>
+          <t>{'19', '41'}</t>
         </is>
       </c>
     </row>
@@ -24185,7 +24185,7 @@
       <c r="M426" t="inlineStr"/>
       <c r="N426" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -24241,7 +24241,7 @@
       <c r="M427" t="inlineStr"/>
       <c r="N427" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -24297,7 +24297,7 @@
       <c r="M428" t="inlineStr"/>
       <c r="N428" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -24353,7 +24353,7 @@
       <c r="M429" t="inlineStr"/>
       <c r="N429" t="inlineStr">
         <is>
-          <t>{'41', '66'}</t>
+          <t>{'66', '41'}</t>
         </is>
       </c>
     </row>
@@ -24413,7 +24413,7 @@
       <c r="M430" t="inlineStr"/>
       <c r="N430" t="inlineStr">
         <is>
-          <t>{'41', '66', '53'}</t>
+          <t>{'66', '41', '53'}</t>
         </is>
       </c>
     </row>
@@ -24629,7 +24629,7 @@
       <c r="M434" t="inlineStr"/>
       <c r="N434" t="inlineStr">
         <is>
-          <t>{'49', '41', '47', '53'}</t>
+          <t>{'47', '49', '41', '53'}</t>
         </is>
       </c>
     </row>
@@ -24957,7 +24957,7 @@
       <c r="M440" t="inlineStr"/>
       <c r="N440" t="inlineStr">
         <is>
-          <t>{'41', '47'}</t>
+          <t>{'47', '41'}</t>
         </is>
       </c>
     </row>
@@ -25013,7 +25013,7 @@
       <c r="M441" t="inlineStr"/>
       <c r="N441" t="inlineStr">
         <is>
-          <t>{'41', '47'}</t>
+          <t>{'47', '41'}</t>
         </is>
       </c>
     </row>
@@ -25121,7 +25121,7 @@
       <c r="M443" t="inlineStr"/>
       <c r="N443" t="inlineStr">
         <is>
-          <t>{'41', '54', '50'}</t>
+          <t>{'50', '41', '54'}</t>
         </is>
       </c>
     </row>
@@ -25177,7 +25177,7 @@
       <c r="M444" t="inlineStr"/>
       <c r="N444" t="inlineStr">
         <is>
-          <t>{'41', '47'}</t>
+          <t>{'47', '41'}</t>
         </is>
       </c>
     </row>
@@ -25509,7 +25509,7 @@
       <c r="M450" t="inlineStr"/>
       <c r="N450" t="inlineStr">
         <is>
-          <t>{'49', '41', '47', '53'}</t>
+          <t>{'47', '49', '41', '53'}</t>
         </is>
       </c>
     </row>
@@ -25725,7 +25725,7 @@
       <c r="M454" t="inlineStr"/>
       <c r="N454" t="inlineStr">
         <is>
-          <t>{'41', '66', '53'}</t>
+          <t>{'66', '41', '53'}</t>
         </is>
       </c>
     </row>
@@ -25781,7 +25781,7 @@
       <c r="M455" t="inlineStr"/>
       <c r="N455" t="inlineStr">
         <is>
-          <t>{'41', '66'}</t>
+          <t>{'66', '41'}</t>
         </is>
       </c>
     </row>
@@ -25837,7 +25837,7 @@
       <c r="M456" t="inlineStr"/>
       <c r="N456" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -25893,7 +25893,7 @@
       <c r="M457" t="inlineStr"/>
       <c r="N457" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -25949,7 +25949,7 @@
       <c r="M458" t="inlineStr"/>
       <c r="N458" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -26425,7 +26425,7 @@
       </c>
       <c r="N467" t="inlineStr">
         <is>
-          <t>{'41', '19'}</t>
+          <t>{'19', '41'}</t>
         </is>
       </c>
     </row>
@@ -26481,7 +26481,7 @@
       </c>
       <c r="N468" t="inlineStr">
         <is>
-          <t>{'41', '19'}</t>
+          <t>{'19', '41'}</t>
         </is>
       </c>
     </row>
@@ -26537,7 +26537,7 @@
       </c>
       <c r="N469" t="inlineStr">
         <is>
-          <t>{'41', '19'}</t>
+          <t>{'19', '41'}</t>
         </is>
       </c>
     </row>
@@ -26593,7 +26593,7 @@
       <c r="M470" t="inlineStr"/>
       <c r="N470" t="inlineStr">
         <is>
-          <t>{'43', '246'}</t>
+          <t>{'246', '43'}</t>
         </is>
       </c>
     </row>
@@ -26653,7 +26653,7 @@
       </c>
       <c r="N471" t="inlineStr">
         <is>
-          <t>{'43', '246', '26'}</t>
+          <t>{'246', '26', '43'}</t>
         </is>
       </c>
     </row>
@@ -26709,7 +26709,7 @@
       <c r="M472" t="inlineStr"/>
       <c r="N472" t="inlineStr">
         <is>
-          <t>{'43', '246'}</t>
+          <t>{'246', '43'}</t>
         </is>
       </c>
     </row>
@@ -26765,7 +26765,7 @@
       <c r="M473" t="inlineStr"/>
       <c r="N473" t="inlineStr">
         <is>
-          <t>{'43', '246'}</t>
+          <t>{'246', '43'}</t>
         </is>
       </c>
     </row>
@@ -26825,7 +26825,7 @@
       </c>
       <c r="N474" t="inlineStr">
         <is>
-          <t>{'43', '246', '65', '7'}</t>
+          <t>{'246', '43', '7', '65'}</t>
         </is>
       </c>
     </row>
@@ -26937,7 +26937,7 @@
       <c r="M476" t="inlineStr"/>
       <c r="N476" t="inlineStr">
         <is>
-          <t>{'21', '54', '48', '53', '18', '43', '22', '52', '51'}</t>
+          <t>{'22', '54', '53', '48', '18', '51', '21', '52', '43'}</t>
         </is>
       </c>
     </row>
@@ -26997,7 +26997,7 @@
       <c r="M477" t="inlineStr"/>
       <c r="N477" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -27053,7 +27053,7 @@
       <c r="M478" t="inlineStr"/>
       <c r="N478" t="inlineStr">
         <is>
-          <t>{'47', '66', '44'}</t>
+          <t>{'66', '47', '44'}</t>
         </is>
       </c>
     </row>
@@ -27109,7 +27109,7 @@
       <c r="M479" t="inlineStr"/>
       <c r="N479" t="inlineStr">
         <is>
-          <t>{'47', '66', '44'}</t>
+          <t>{'66', '47', '44'}</t>
         </is>
       </c>
     </row>
@@ -27321,7 +27321,7 @@
       <c r="M483" t="inlineStr"/>
       <c r="N483" t="inlineStr">
         <is>
-          <t>{'44', '53'}</t>
+          <t>{'53', '44'}</t>
         </is>
       </c>
     </row>
@@ -28789,7 +28789,7 @@
       <c r="M511" t="inlineStr"/>
       <c r="N511" t="inlineStr">
         <is>
-          <t>{'44', '53'}</t>
+          <t>{'53', '44'}</t>
         </is>
       </c>
     </row>
@@ -29001,7 +29001,7 @@
       <c r="M515" t="inlineStr"/>
       <c r="N515" t="inlineStr">
         <is>
-          <t>{'47', '66', '44'}</t>
+          <t>{'66', '47', '44'}</t>
         </is>
       </c>
     </row>
@@ -29057,7 +29057,7 @@
       <c r="M516" t="inlineStr"/>
       <c r="N516" t="inlineStr">
         <is>
-          <t>{'47', '66', '44'}</t>
+          <t>{'66', '47', '44'}</t>
         </is>
       </c>
     </row>
@@ -29117,7 +29117,7 @@
       <c r="M517" t="inlineStr"/>
       <c r="N517" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -29225,7 +29225,7 @@
       <c r="M519" t="inlineStr"/>
       <c r="N519" t="inlineStr">
         <is>
-          <t>{'62', '464', '461'}</t>
+          <t>{'464', '461', '62'}</t>
         </is>
       </c>
     </row>
@@ -29397,7 +29397,7 @@
       </c>
       <c r="N522" t="inlineStr">
         <is>
-          <t>{'25', '5', '463', '461'}</t>
+          <t>{'463', '25', '5', '461'}</t>
         </is>
       </c>
     </row>
@@ -29457,7 +29457,7 @@
       </c>
       <c r="N523" t="inlineStr">
         <is>
-          <t>{'62', '246', '24', '461'}</t>
+          <t>{'246', '461', '24', '62'}</t>
         </is>
       </c>
     </row>
@@ -29993,7 +29993,7 @@
       </c>
       <c r="N533" t="inlineStr">
         <is>
-          <t>{'25', '5', '463'}</t>
+          <t>{'463', '25', '5'}</t>
         </is>
       </c>
     </row>
@@ -30365,7 +30365,7 @@
       <c r="M540" t="inlineStr"/>
       <c r="N540" t="inlineStr">
         <is>
-          <t>{'62', '464', '461'}</t>
+          <t>{'464', '461', '62'}</t>
         </is>
       </c>
     </row>
@@ -30425,7 +30425,7 @@
       <c r="M541" t="inlineStr"/>
       <c r="N541" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -30589,7 +30589,7 @@
       <c r="M544" t="inlineStr"/>
       <c r="N544" t="inlineStr">
         <is>
-          <t>{'49', '47', '53'}</t>
+          <t>{'47', '49', '53'}</t>
         </is>
       </c>
     </row>
@@ -30649,7 +30649,7 @@
       <c r="M545" t="inlineStr"/>
       <c r="N545" t="inlineStr">
         <is>
-          <t>{'49', '41', '47', '53'}</t>
+          <t>{'47', '49', '41', '53'}</t>
         </is>
       </c>
     </row>
@@ -30965,7 +30965,7 @@
       <c r="M551" t="inlineStr"/>
       <c r="N551" t="inlineStr">
         <is>
-          <t>{'47', '54', '50'}</t>
+          <t>{'47', '50', '54'}</t>
         </is>
       </c>
     </row>
@@ -31281,7 +31281,7 @@
       <c r="M557" t="inlineStr"/>
       <c r="N557" t="inlineStr">
         <is>
-          <t>{'47', '54', '50'}</t>
+          <t>{'47', '50', '54'}</t>
         </is>
       </c>
     </row>
@@ -31441,7 +31441,7 @@
       <c r="M560" t="inlineStr"/>
       <c r="N560" t="inlineStr">
         <is>
-          <t>{'41', '47'}</t>
+          <t>{'47', '41'}</t>
         </is>
       </c>
     </row>
@@ -31601,7 +31601,7 @@
       <c r="M563" t="inlineStr"/>
       <c r="N563" t="inlineStr">
         <is>
-          <t>{'47', '54', '50'}</t>
+          <t>{'47', '50', '54'}</t>
         </is>
       </c>
     </row>
@@ -31917,7 +31917,7 @@
       <c r="M569" t="inlineStr"/>
       <c r="N569" t="inlineStr">
         <is>
-          <t>{'47', '54', '50'}</t>
+          <t>{'47', '50', '54'}</t>
         </is>
       </c>
     </row>
@@ -32341,7 +32341,7 @@
       <c r="M577" t="inlineStr"/>
       <c r="N577" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -33597,7 +33597,7 @@
       <c r="M601" t="inlineStr"/>
       <c r="N601" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -33657,7 +33657,7 @@
       <c r="M602" t="inlineStr"/>
       <c r="N602" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -34449,7 +34449,7 @@
       </c>
       <c r="N617" t="inlineStr">
         <is>
-          <t>{'61', '19', '36', '22', '369', '231', '15', '51', '50'}</t>
+          <t>{'22', '231', '19', '369', '15', '61', '51', '50', '36'}</t>
         </is>
       </c>
     </row>
@@ -35141,7 +35141,7 @@
       </c>
       <c r="N630" t="inlineStr">
         <is>
-          <t>{'2', '15', '62'}</t>
+          <t>{'15', '2', '62'}</t>
         </is>
       </c>
     </row>
@@ -35253,7 +35253,7 @@
       </c>
       <c r="N632" t="inlineStr">
         <is>
-          <t>{'24', '62'}</t>
+          <t>{'62', '24'}</t>
         </is>
       </c>
     </row>
@@ -35309,7 +35309,7 @@
       </c>
       <c r="N633" t="inlineStr">
         <is>
-          <t>{'24', '62'}</t>
+          <t>{'62', '24'}</t>
         </is>
       </c>
     </row>
@@ -35373,7 +35373,7 @@
       </c>
       <c r="N634" t="inlineStr">
         <is>
-          <t>{'24', '62', '2', '50', '246', '15', '51'}</t>
+          <t>{'24', '15', '62', '246', '51', '50', '2'}</t>
         </is>
       </c>
     </row>
@@ -35433,7 +35433,7 @@
       </c>
       <c r="N635" t="inlineStr">
         <is>
-          <t>{'246', '24', '62'}</t>
+          <t>{'246', '62', '24'}</t>
         </is>
       </c>
     </row>
@@ -35493,7 +35493,7 @@
       </c>
       <c r="N636" t="inlineStr">
         <is>
-          <t>{'62', '246', '24', '461'}</t>
+          <t>{'246', '461', '24', '62'}</t>
         </is>
       </c>
     </row>
@@ -35553,7 +35553,7 @@
       </c>
       <c r="N637" t="inlineStr">
         <is>
-          <t>{'62', '25', '65', '5', '15'}</t>
+          <t>{'25', '15', '62', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -35825,7 +35825,7 @@
       </c>
       <c r="N642" t="inlineStr">
         <is>
-          <t>{'50', '4', '51', '62'}</t>
+          <t>{'4', '50', '51', '62'}</t>
         </is>
       </c>
     </row>
@@ -35945,7 +35945,7 @@
       </c>
       <c r="N644" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -36057,7 +36057,7 @@
       </c>
       <c r="N646" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -36117,7 +36117,7 @@
       </c>
       <c r="N647" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -36177,7 +36177,7 @@
       </c>
       <c r="N648" t="inlineStr">
         <is>
-          <t>{'62', '65', '12', '245'}</t>
+          <t>{'65', '12', '245', '62'}</t>
         </is>
       </c>
     </row>
@@ -36237,7 +36237,7 @@
       <c r="M649" t="inlineStr"/>
       <c r="N649" t="inlineStr">
         <is>
-          <t>{'40', '245', '54', '53', '62', '240', '37', '65', '51'}</t>
+          <t>{'240', '54', '245', '53', '62', '37', '51', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -36349,7 +36349,7 @@
       </c>
       <c r="N651" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -36469,7 +36469,7 @@
       </c>
       <c r="N653" t="inlineStr">
         <is>
-          <t>{'50', '4', '51', '62'}</t>
+          <t>{'4', '50', '51', '62'}</t>
         </is>
       </c>
     </row>
@@ -36797,7 +36797,7 @@
       </c>
       <c r="N659" t="inlineStr">
         <is>
-          <t>{'62', '246', '24', '461'}</t>
+          <t>{'246', '461', '24', '62'}</t>
         </is>
       </c>
     </row>
@@ -36857,7 +36857,7 @@
       </c>
       <c r="N660" t="inlineStr">
         <is>
-          <t>{'246', '24', '62'}</t>
+          <t>{'246', '62', '24'}</t>
         </is>
       </c>
     </row>
@@ -36913,7 +36913,7 @@
       </c>
       <c r="N661" t="inlineStr">
         <is>
-          <t>{'24', '62'}</t>
+          <t>{'62', '24'}</t>
         </is>
       </c>
     </row>
@@ -36969,7 +36969,7 @@
       </c>
       <c r="N662" t="inlineStr">
         <is>
-          <t>{'24', '62'}</t>
+          <t>{'62', '24'}</t>
         </is>
       </c>
     </row>
@@ -37029,7 +37029,7 @@
       </c>
       <c r="N663" t="inlineStr">
         <is>
-          <t>{'2', '15', '62'}</t>
+          <t>{'15', '2', '62'}</t>
         </is>
       </c>
     </row>
@@ -37349,7 +37349,7 @@
       </c>
       <c r="N669" t="inlineStr">
         <is>
-          <t>{'1', '63'}</t>
+          <t>{'63', '1'}</t>
         </is>
       </c>
     </row>
@@ -38241,7 +38241,7 @@
       <c r="M686" t="inlineStr"/>
       <c r="N686" t="inlineStr">
         <is>
-          <t>{'369', '61', '63'}</t>
+          <t>{'369', '63', '61'}</t>
         </is>
       </c>
     </row>
@@ -38557,7 +38557,7 @@
       </c>
       <c r="N692" t="inlineStr">
         <is>
-          <t>{'1', '63'}</t>
+          <t>{'63', '1'}</t>
         </is>
       </c>
     </row>
@@ -38717,7 +38717,7 @@
       <c r="M695" t="inlineStr"/>
       <c r="N695" t="inlineStr">
         <is>
-          <t>{'43', '246', '65'}</t>
+          <t>{'246', '43', '65'}</t>
         </is>
       </c>
     </row>
@@ -38937,7 +38937,7 @@
       </c>
       <c r="N699" t="inlineStr">
         <is>
-          <t>{'62', '65', '12', '245'}</t>
+          <t>{'65', '12', '245', '62'}</t>
         </is>
       </c>
     </row>
@@ -38997,7 +38997,7 @@
       </c>
       <c r="N700" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -39109,7 +39109,7 @@
       </c>
       <c r="N702" t="inlineStr">
         <is>
-          <t>{'5', '246', '15', '65'}</t>
+          <t>{'246', '15', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -39169,7 +39169,7 @@
       </c>
       <c r="N703" t="inlineStr">
         <is>
-          <t>{'62', '25', '65', '5', '15'}</t>
+          <t>{'25', '15', '62', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -39229,7 +39229,7 @@
       </c>
       <c r="N704" t="inlineStr">
         <is>
-          <t>{'5', '246', '15', '65'}</t>
+          <t>{'246', '15', '5', '65'}</t>
         </is>
       </c>
     </row>
@@ -39289,7 +39289,7 @@
       </c>
       <c r="N705" t="inlineStr">
         <is>
-          <t>{'5', '246', '65', '24'}</t>
+          <t>{'246', '5', '24', '65'}</t>
         </is>
       </c>
     </row>
@@ -39405,7 +39405,7 @@
       </c>
       <c r="N707" t="inlineStr">
         <is>
-          <t>{'246', '65', '12'}</t>
+          <t>{'12', '246', '65'}</t>
         </is>
       </c>
     </row>
@@ -39521,7 +39521,7 @@
       </c>
       <c r="N709" t="inlineStr">
         <is>
-          <t>{'52', '65', '4', '245'}</t>
+          <t>{'52', '4', '245', '65'}</t>
         </is>
       </c>
     </row>
@@ -39581,7 +39581,7 @@
       </c>
       <c r="N710" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -39641,7 +39641,7 @@
       </c>
       <c r="N711" t="inlineStr">
         <is>
-          <t>{'12', '245', '62', '65', '4'}</t>
+          <t>{'245', '62', '4', '65', '12'}</t>
         </is>
       </c>
     </row>
@@ -39701,7 +39701,7 @@
       </c>
       <c r="N712" t="inlineStr">
         <is>
-          <t>{'62', '65', '12', '245'}</t>
+          <t>{'65', '12', '245', '62'}</t>
         </is>
       </c>
     </row>
@@ -39761,7 +39761,7 @@
       <c r="M713" t="inlineStr"/>
       <c r="N713" t="inlineStr">
         <is>
-          <t>{'40', '245', '54', '53', '62', '240', '37', '65', '51'}</t>
+          <t>{'240', '54', '245', '53', '62', '37', '51', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -39817,7 +39817,7 @@
       <c r="M714" t="inlineStr"/>
       <c r="N714" t="inlineStr">
         <is>
-          <t>{'40', '245', '37', '240', '65'}</t>
+          <t>{'240', '245', '37', '65', '40'}</t>
         </is>
       </c>
     </row>
@@ -39985,7 +39985,7 @@
       </c>
       <c r="N717" t="inlineStr">
         <is>
-          <t>{'14', '65', '22'}</t>
+          <t>{'22', '14', '65'}</t>
         </is>
       </c>
     </row>
@@ -40041,7 +40041,7 @@
       <c r="M718" t="inlineStr"/>
       <c r="N718" t="inlineStr">
         <is>
-          <t>{'65', '22'}</t>
+          <t>{'22', '65'}</t>
         </is>
       </c>
     </row>
@@ -40097,7 +40097,7 @@
       <c r="M719" t="inlineStr"/>
       <c r="N719" t="inlineStr">
         <is>
-          <t>{'65', '22'}</t>
+          <t>{'22', '65'}</t>
         </is>
       </c>
     </row>
@@ -40153,7 +40153,7 @@
       <c r="M720" t="inlineStr"/>
       <c r="N720" t="inlineStr">
         <is>
-          <t>{'43', '246', '65'}</t>
+          <t>{'246', '43', '65'}</t>
         </is>
       </c>
     </row>
@@ -40949,7 +40949,7 @@
       <c r="M735" t="inlineStr"/>
       <c r="N735" t="inlineStr">
         <is>
-          <t>{'41', '66'}</t>
+          <t>{'66', '41'}</t>
         </is>
       </c>
     </row>
@@ -41005,7 +41005,7 @@
       <c r="M736" t="inlineStr"/>
       <c r="N736" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -41061,7 +41061,7 @@
       <c r="M737" t="inlineStr"/>
       <c r="N737" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -41117,7 +41117,7 @@
       <c r="M738" t="inlineStr"/>
       <c r="N738" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -41177,7 +41177,7 @@
       <c r="M739" t="inlineStr"/>
       <c r="N739" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -41237,7 +41237,7 @@
       <c r="M740" t="inlineStr"/>
       <c r="N740" t="inlineStr">
         <is>
-          <t>{'54', '44', '49', '47', '50', '66'}</t>
+          <t>{'54', '49', '47', '44', '66', '50'}</t>
         </is>
       </c>
     </row>
@@ -41293,7 +41293,7 @@
       <c r="M741" t="inlineStr"/>
       <c r="N741" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -41349,7 +41349,7 @@
       <c r="M742" t="inlineStr"/>
       <c r="N742" t="inlineStr">
         <is>
-          <t>{'41', '66', '47'}</t>
+          <t>{'66', '47', '41'}</t>
         </is>
       </c>
     </row>
@@ -41405,7 +41405,7 @@
       <c r="M743" t="inlineStr"/>
       <c r="N743" t="inlineStr">
         <is>
-          <t>{'41', '66'}</t>
+          <t>{'66', '41'}</t>
         </is>
       </c>
     </row>
@@ -41465,7 +41465,7 @@
       <c r="M744" t="inlineStr"/>
       <c r="N744" t="inlineStr">
         <is>
-          <t>{'41', '66', '53'}</t>
+          <t>{'66', '41', '53'}</t>
         </is>
       </c>
     </row>
@@ -42049,7 +42049,7 @@
       <c r="M755" t="inlineStr"/>
       <c r="N755" t="inlineStr">
         <is>
-          <t>{'68', '267'}</t>
+          <t>{'267', '68'}</t>
         </is>
       </c>
     </row>
@@ -42105,7 +42105,7 @@
       <c r="M756" t="inlineStr"/>
       <c r="N756" t="inlineStr">
         <is>
-          <t>{'68', '267'}</t>
+          <t>{'267', '68'}</t>
         </is>
       </c>
     </row>
@@ -42213,7 +42213,7 @@
       <c r="M758" t="inlineStr"/>
       <c r="N758" t="inlineStr">
         <is>
-          <t>{'68', '50', '51'}</t>
+          <t>{'50', '51', '68'}</t>
         </is>
       </c>
     </row>

</xml_diff>